<commit_message>
starting bam file transfer work
</commit_message>
<xml_diff>
--- a/project management/gantt chart - moved to drive.xlsx
+++ b/project management/gantt chart - moved to drive.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28320" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="306">
   <si>
     <t>TAU data</t>
   </si>
@@ -54,15 +54,6 @@
     <t>MayoLOADGWAS Exome sequencing</t>
   </si>
   <si>
-    <t>Public Synapse ID - data</t>
-  </si>
-  <si>
-    <t>Public Synapse ID - study info</t>
-  </si>
-  <si>
-    <t>Working Synapse ID - data</t>
-  </si>
-  <si>
     <t>syn3157175</t>
   </si>
   <si>
@@ -504,9 +495,6 @@
     <t>I think this is my public root directory. (not sure of working id)</t>
   </si>
   <si>
-    <t>Working Synapse ID - study info</t>
-  </si>
-  <si>
     <t>syn3163039</t>
   </si>
   <si>
@@ -934,6 +922,21 @@
   </si>
   <si>
     <t>syn3910665</t>
+  </si>
+  <si>
+    <t>Partner Page Synapse ID - study info</t>
+  </si>
+  <si>
+    <t>Partner Page Synapse ID - data</t>
+  </si>
+  <si>
+    <t>Knowledge Bank Synapse ID - study info</t>
+  </si>
+  <si>
+    <t>Knowledge Bank Synapse ID - data</t>
+  </si>
+  <si>
+    <t>`</t>
   </si>
 </sst>
 </file>
@@ -1091,7 +1094,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="121">
+  <cellStyleXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1174,6 +1177,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1260,7 +1265,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="17" fontId="1" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="121">
+  <cellStyles count="123">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Check Cell" xfId="56" builtinId="23"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -1366,6 +1371,8 @@
     <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="119" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="121" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="81" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="24" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
@@ -3921,10 +3928,10 @@
   <dimension ref="A1:I144"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C28" sqref="C28"/>
+      <selection pane="bottomRight" activeCell="F138" sqref="F138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3935,66 +3942,66 @@
     <col min="9" max="9" width="68.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="45">
+    <row r="1" spans="1:9" ht="60">
       <c r="A1" s="3" t="s">
-        <v>11</v>
+        <v>304</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>12</v>
+        <v>303</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>13</v>
+        <v>302</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>161</v>
+        <v>301</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
       </c>
       <c r="I1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="B2" t="s">
+        <v>154</v>
+      </c>
+      <c r="D2" t="s">
+        <v>156</v>
+      </c>
+      <c r="H2" t="s">
+        <v>155</v>
+      </c>
+      <c r="I2" t="s">
         <v>157</v>
-      </c>
-      <c r="D2" t="s">
-        <v>159</v>
-      </c>
-      <c r="H2" t="s">
-        <v>158</v>
-      </c>
-      <c r="I2" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="B4" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="D4" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="F4" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="G4" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="I4" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="E6" s="1">
         <v>42036</v>
@@ -4003,49 +4010,52 @@
         <v>9</v>
       </c>
       <c r="G6" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="E7" s="1"/>
       <c r="H7" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E8" s="1"/>
       <c r="H8" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="I8" s="7"/>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E9" s="1"/>
       <c r="H9" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="I9" s="7"/>
     </row>
     <row r="10" spans="1:9">
+      <c r="A10" t="s">
+        <v>305</v>
+      </c>
       <c r="E10" s="1"/>
       <c r="H10" s="5"/>
       <c r="I10" s="7"/>
     </row>
     <row r="11" spans="1:9">
       <c r="B11" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D11" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E11" s="2">
         <v>42050</v>
@@ -4054,282 +4064,282 @@
         <v>3</v>
       </c>
       <c r="G11" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="H11" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="I11" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="B12" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D12" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="G12" t="s">
         <v>0</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="I12" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C13" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="H13" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="C14" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="I14" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C15" s="23" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="H15" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="I15" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C16" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="H16" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C17" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H17" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C18" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I18" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="19" spans="1:9" s="8" customFormat="1">
       <c r="A19" s="8" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H19" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="20" spans="1:9" s="8" customFormat="1">
       <c r="C20" s="23" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="H20" s="23" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="21" spans="1:9" s="8" customFormat="1">
       <c r="C21" s="23" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="H21" s="23" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C22" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H22" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C23" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="H23" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C24" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="I24" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="25" spans="1:9" s="8" customFormat="1">
       <c r="C25" s="8" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="H25" s="8" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
     </row>
     <row r="26" spans="1:9" s="8" customFormat="1">
       <c r="A26" s="8" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="H26" s="8" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="27" spans="1:9" s="8" customFormat="1">
       <c r="C27" s="23" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="H27" s="8" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
     </row>
     <row r="28" spans="1:9" s="8" customFormat="1" ht="16" thickBot="1">
       <c r="C28" s="23" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="H28" s="8" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
     </row>
     <row r="29" spans="1:9" s="9" customFormat="1" ht="17" thickTop="1" thickBot="1">
       <c r="E29" s="9" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="H29" s="9" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="16" thickTop="1"/>
     <row r="31" spans="1:9" s="23" customFormat="1">
       <c r="D31" s="23" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="G31" s="23" t="s">
         <v>1</v>
       </c>
       <c r="H31" s="23" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="32" spans="1:9" s="8" customFormat="1">
       <c r="C32" s="8" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="H32" s="8" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="I32" s="8" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="33" spans="1:9" s="23" customFormat="1">
       <c r="C33" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="H33" s="23" t="s">
         <v>149</v>
-      </c>
-      <c r="H33" s="23" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="34" spans="1:9" s="23" customFormat="1">
       <c r="C34" s="23" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H34" s="23" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="35" spans="1:9" s="23" customFormat="1">
       <c r="C35" s="23" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="H35" s="23" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="36" spans="1:9" s="23" customFormat="1">
       <c r="C36" s="23" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="H36" s="23" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="37" spans="1:9" s="23" customFormat="1" ht="16" thickBot="1">
       <c r="C37" s="23" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="H37" s="23" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="38" spans="1:9" s="9" customFormat="1" ht="17" thickTop="1" thickBot="1">
       <c r="E38" s="9" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="H38" s="9" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="16" thickTop="1"/>
     <row r="40" spans="1:9">
       <c r="B40" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E40" s="2">
         <v>42050</v>
@@ -4338,115 +4348,115 @@
         <v>5</v>
       </c>
       <c r="I40" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="30">
       <c r="B41" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E41" s="2"/>
       <c r="G41" s="5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="42" spans="1:9">
       <c r="A42" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C42" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E42" s="2"/>
       <c r="H42" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="I42" s="7"/>
     </row>
     <row r="43" spans="1:9">
       <c r="A43" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C43" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E43" s="2"/>
       <c r="H43" s="5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="I43" s="7"/>
     </row>
     <row r="44" spans="1:9">
       <c r="A44" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C44" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E44" s="2"/>
       <c r="H44" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="45" spans="1:9">
       <c r="A45" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C45" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E45" s="2"/>
       <c r="H45" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="I45" s="7"/>
     </row>
     <row r="46" spans="1:9" ht="30">
       <c r="B46" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E46" s="2"/>
       <c r="G46" s="5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="I46" s="7"/>
     </row>
     <row r="47" spans="1:9">
       <c r="A47" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C47" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E47" s="2"/>
       <c r="H47" s="5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="I47" s="7"/>
     </row>
     <row r="48" spans="1:9">
       <c r="A48" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C48" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E48" s="2"/>
       <c r="H48" s="5" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="I48" s="7"/>
     </row>
     <row r="49" spans="1:9">
       <c r="A49" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C49" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E49" s="2"/>
       <c r="H49" s="5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="I49" s="7"/>
     </row>
@@ -4457,7 +4467,7 @@
     </row>
     <row r="51" spans="1:9">
       <c r="B51" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E51" s="2">
         <v>42050</v>
@@ -4468,120 +4478,120 @@
     </row>
     <row r="52" spans="1:9">
       <c r="A52" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E52" s="2"/>
       <c r="H52" s="5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="53" spans="1:9">
       <c r="A53" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E53" s="2"/>
       <c r="H53" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="I53" s="7"/>
     </row>
     <row r="54" spans="1:9">
       <c r="A54" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E54" s="2"/>
       <c r="H54" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="I54" s="7"/>
     </row>
     <row r="55" spans="1:9">
       <c r="A55" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E55" s="2"/>
       <c r="H55" s="5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="I55" s="7"/>
     </row>
     <row r="56" spans="1:9">
       <c r="A56" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E56" s="2"/>
       <c r="H56" s="5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I56" s="7"/>
     </row>
     <row r="57" spans="1:9">
       <c r="A57" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E57" s="2"/>
       <c r="H57" s="5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="I57" s="7"/>
     </row>
     <row r="58" spans="1:9">
       <c r="A58" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E58" s="2"/>
       <c r="H58" s="5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="I58" s="7"/>
     </row>
     <row r="59" spans="1:9">
       <c r="A59" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E59" s="2"/>
       <c r="H59" s="5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="I59" s="7"/>
     </row>
     <row r="60" spans="1:9">
       <c r="A60" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="E60" s="2"/>
       <c r="H60" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="I60" s="7"/>
     </row>
     <row r="61" spans="1:9">
       <c r="A61" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E61" s="2"/>
       <c r="H61" s="5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I61" s="7"/>
     </row>
     <row r="62" spans="1:9">
       <c r="A62" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E62" s="2"/>
       <c r="H62" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="I62" s="7"/>
     </row>
     <row r="63" spans="1:9">
       <c r="A63" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E63" s="2"/>
       <c r="H63" s="5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="I63" s="7"/>
     </row>
@@ -4598,7 +4608,7 @@
         <v>10</v>
       </c>
       <c r="I65" s="9" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="66" spans="1:9" ht="16" thickTop="1">
@@ -4607,21 +4617,21 @@
     </row>
     <row r="67" spans="1:9">
       <c r="B67" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="D67" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="E67" s="1"/>
       <c r="F67" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="G67" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="H67" s="5"/>
       <c r="I67" s="7" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
     </row>
     <row r="68" spans="1:9">
@@ -4629,7 +4639,7 @@
     </row>
     <row r="69" spans="1:9">
       <c r="B69" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E69" s="2">
         <v>42050</v>
@@ -4640,50 +4650,50 @@
     </row>
     <row r="70" spans="1:9">
       <c r="A70" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C70" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E70" s="2"/>
       <c r="H70" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="71" spans="1:9">
       <c r="A71" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C71" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E71" s="2"/>
       <c r="H71" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="72" spans="1:9">
       <c r="A72" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C72" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E72" s="2"/>
       <c r="H72" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="73" spans="1:9">
       <c r="A73" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C73" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E73" s="2"/>
       <c r="H73" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="74" spans="1:9">
@@ -4691,10 +4701,10 @@
     </row>
     <row r="75" spans="1:9" s="11" customFormat="1">
       <c r="B75" s="11" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D75" s="23" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="E75" s="12">
         <v>42036</v>
@@ -4707,193 +4717,193 @@
       </c>
       <c r="H75"/>
       <c r="I75" s="11" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="76" spans="1:9" s="15" customFormat="1">
       <c r="D76" s="15" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="E76" s="16"/>
       <c r="I76" s="15" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="77" spans="1:9" s="11" customFormat="1">
       <c r="A77" s="11" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E77" s="12"/>
       <c r="H77" s="13" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="78" spans="1:9" s="15" customFormat="1">
       <c r="C78" s="23" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="E78" s="16"/>
       <c r="H78" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
     </row>
     <row r="79" spans="1:9" s="11" customFormat="1">
       <c r="A79" s="11" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C79" s="11" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="E79" s="12"/>
       <c r="H79" s="14" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="I79" s="11" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
     </row>
     <row r="80" spans="1:9" s="26" customFormat="1">
       <c r="C80" s="26" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="E80" s="27"/>
       <c r="H80" s="26" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
     </row>
     <row r="81" spans="1:9" s="15" customFormat="1">
       <c r="C81" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="E81" s="16"/>
       <c r="H81" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
     </row>
     <row r="82" spans="1:9" s="11" customFormat="1">
       <c r="A82" s="11" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="E82" s="12"/>
       <c r="H82" s="13" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="83" spans="1:9" s="4" customFormat="1">
       <c r="C83" s="4" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="E83" s="6"/>
       <c r="H83" s="4" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="84" spans="1:9" s="15" customFormat="1">
       <c r="C84" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="E84" s="16"/>
       <c r="H84" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
     </row>
     <row r="85" spans="1:9" s="11" customFormat="1">
       <c r="A85" s="11" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C85" s="11" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="E85" s="12"/>
       <c r="H85" s="14" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="86" spans="1:9" s="4" customFormat="1">
       <c r="C86" s="4" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="E86" s="6"/>
       <c r="H86" s="4" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
     </row>
     <row r="87" spans="1:9" s="11" customFormat="1">
       <c r="A87" s="11" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C87" s="11" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="E87" s="12"/>
       <c r="H87" s="14" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="88" spans="1:9" s="15" customFormat="1">
       <c r="C88" s="15" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="E88" s="16"/>
       <c r="H88" s="15" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
     </row>
     <row r="89" spans="1:9" s="15" customFormat="1">
       <c r="C89" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="E89" s="16"/>
       <c r="H89" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
     </row>
     <row r="90" spans="1:9" s="11" customFormat="1">
       <c r="A90" s="11" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E90" s="12"/>
       <c r="H90" s="13" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="91" spans="1:9" s="15" customFormat="1">
       <c r="C91" s="15" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="E91" s="16"/>
       <c r="H91" s="15" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="92" spans="1:9" s="15" customFormat="1">
       <c r="C92" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="E92" s="16"/>
       <c r="H92" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
     </row>
     <row r="93" spans="1:9" s="11" customFormat="1">
       <c r="A93" s="11" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C93" s="11" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="E93" s="12"/>
       <c r="H93" s="14" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="94" spans="1:9" s="4" customFormat="1">
       <c r="C94" s="4" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E94" s="6"/>
       <c r="H94" s="4" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
     <row r="95" spans="1:9" s="17" customFormat="1">
@@ -4902,192 +4912,192 @@
     </row>
     <row r="96" spans="1:9" s="15" customFormat="1">
       <c r="D96" s="15" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E96" s="16"/>
       <c r="H96" s="20"/>
       <c r="I96" s="15" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="97" spans="1:9" s="15" customFormat="1">
       <c r="C97" s="15" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="E97" s="16"/>
       <c r="H97" s="21" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
     </row>
     <row r="98" spans="1:9" s="15" customFormat="1">
       <c r="C98" s="15" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="E98" s="16"/>
       <c r="H98" s="21" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="99" spans="1:9" s="11" customFormat="1">
       <c r="A99" s="11" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="E99" s="12"/>
       <c r="H99" s="13" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="I99" s="11" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
     </row>
     <row r="100" spans="1:9" s="15" customFormat="1">
       <c r="C100" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="E100" s="16"/>
       <c r="H100" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="101" spans="1:9" s="11" customFormat="1">
       <c r="A101" s="11" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C101" s="11" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="E101" s="12"/>
       <c r="H101" s="14" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="I101" s="11" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
     </row>
     <row r="102" spans="1:9" s="15" customFormat="1">
       <c r="C102" s="15" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="E102" s="16"/>
       <c r="H102" s="22" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="103" spans="1:9" s="15" customFormat="1">
       <c r="C103" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="E103" s="16"/>
       <c r="H103" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
     </row>
     <row r="104" spans="1:9" s="11" customFormat="1">
       <c r="A104" s="11" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E104" s="12"/>
       <c r="H104" s="13" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="105" spans="1:9" s="15" customFormat="1">
       <c r="C105" s="15" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="E105" s="16"/>
       <c r="H105" s="15" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="106" spans="1:9" s="15" customFormat="1">
       <c r="C106" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="E106" s="16"/>
       <c r="H106" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
     </row>
     <row r="107" spans="1:9" s="11" customFormat="1">
       <c r="A107" s="11" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C107" s="11" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="E107" s="12"/>
       <c r="H107" s="14" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="108" spans="1:9" s="11" customFormat="1">
       <c r="A108" s="11" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C108" s="11" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="E108" s="12"/>
       <c r="H108" s="14" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="109" spans="1:9" s="15" customFormat="1">
       <c r="C109" s="15" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="E109" s="16"/>
       <c r="H109" s="22" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="110" spans="1:9" s="15" customFormat="1">
       <c r="C110" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="E110" s="16"/>
       <c r="H110" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="111" spans="1:9" s="11" customFormat="1">
       <c r="A111" s="11" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E111" s="12"/>
       <c r="H111" s="13" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="112" spans="1:9" s="15" customFormat="1">
       <c r="C112" s="15" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="E112" s="16"/>
       <c r="H112" s="15" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="113" spans="1:9" s="15" customFormat="1">
       <c r="C113" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="E113" s="16"/>
       <c r="H113" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
     </row>
     <row r="114" spans="1:9" s="11" customFormat="1">
       <c r="A114" s="11" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C114" s="11" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="E114" s="12"/>
       <c r="H114" s="14" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="115" spans="1:9" s="15" customFormat="1" ht="16" thickBot="1">
@@ -5096,10 +5106,10 @@
     </row>
     <row r="116" spans="1:9" s="9" customFormat="1" ht="17" thickTop="1" thickBot="1">
       <c r="E116" s="9" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="H116" s="9" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="117" spans="1:9" ht="16" thickTop="1">
@@ -5109,84 +5119,84 @@
     </row>
     <row r="118" spans="1:9" s="4" customFormat="1">
       <c r="D118" s="4" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="E118" s="6">
         <v>42125</v>
       </c>
       <c r="F118" s="4" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="G118" t="s">
         <v>8</v>
       </c>
       <c r="I118" s="4" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="119" spans="1:9" s="23" customFormat="1">
       <c r="C119" s="23" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="E119" s="25"/>
       <c r="H119" s="23" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
     </row>
     <row r="120" spans="1:9" s="8" customFormat="1">
       <c r="C120" s="8" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="E120" s="24"/>
       <c r="H120" s="8" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="I120" s="8" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="121" spans="1:9" s="23" customFormat="1">
       <c r="C121" s="23" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="E121" s="25"/>
       <c r="H121" s="23" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="122" spans="1:9" s="23" customFormat="1">
       <c r="C122" s="23" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="E122" s="25"/>
       <c r="H122" s="23" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
     </row>
     <row r="123" spans="1:9" s="23" customFormat="1">
       <c r="C123" s="23" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="E123" s="25"/>
       <c r="H123" s="23" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
     </row>
     <row r="124" spans="1:9" s="23" customFormat="1" ht="16" thickBot="1">
       <c r="C124" s="23" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="E124" s="25"/>
       <c r="H124" s="23" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
     </row>
     <row r="125" spans="1:9" s="9" customFormat="1" ht="17" thickTop="1" thickBot="1">
       <c r="E125" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="H125" s="9" t="s">
         <v>183</v>
-      </c>
-      <c r="H125" s="9" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="126" spans="1:9" ht="17" thickTop="1" thickBot="1"/>
@@ -5195,10 +5205,10 @@
         <v>42401</v>
       </c>
       <c r="F127" s="9" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="I127" s="9" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="128" spans="1:9" ht="16" thickTop="1">
@@ -5206,130 +5216,130 @@
     </row>
     <row r="129" spans="3:9" s="4" customFormat="1">
       <c r="D129" s="4" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="E129" s="6">
         <v>42125</v>
       </c>
       <c r="F129" s="4" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="G129" s="4" t="s">
         <v>8</v>
       </c>
       <c r="I129" s="4" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
     </row>
     <row r="130" spans="3:9" s="23" customFormat="1">
       <c r="C130" s="23" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="H130" s="23" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
     </row>
     <row r="131" spans="3:9" s="8" customFormat="1">
       <c r="C131" s="8" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="H131" s="8" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="I131" s="8" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="132" spans="3:9" s="23" customFormat="1">
       <c r="C132" s="23" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="H132" s="23" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
     </row>
     <row r="133" spans="3:9" s="23" customFormat="1">
       <c r="C133" s="23" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="H133" s="23" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
     </row>
     <row r="134" spans="3:9" s="23" customFormat="1">
       <c r="C134" s="23" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="H134" s="23" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="135" spans="3:9" s="23" customFormat="1" ht="16" thickBot="1">
       <c r="C135" s="23" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="H135" s="23" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
     </row>
     <row r="136" spans="3:9" s="9" customFormat="1" ht="17" thickTop="1" thickBot="1">
       <c r="E136" s="9" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="H136" s="9" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="I136" s="9" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="137" spans="3:9" ht="17" thickTop="1" thickBot="1"/>
     <row r="138" spans="3:9" s="9" customFormat="1" ht="17" thickTop="1" thickBot="1">
       <c r="D138" s="9" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="E138" s="9" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="F138" s="9" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G138" s="9" t="s">
         <v>8</v>
       </c>
       <c r="I138" s="9" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="139" spans="3:9" s="9" customFormat="1" ht="17" thickTop="1" thickBot="1">
       <c r="H139" s="9" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="140" spans="3:9" s="9" customFormat="1" ht="17" thickTop="1" thickBot="1">
       <c r="H140" s="9" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="141" spans="3:9" s="9" customFormat="1" ht="17" thickTop="1" thickBot="1">
       <c r="H141" s="9" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="142" spans="3:9" s="9" customFormat="1" ht="17" thickTop="1" thickBot="1">
       <c r="H142" s="9" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="I142" s="9" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
     </row>
     <row r="143" spans="3:9" s="9" customFormat="1" ht="17" thickTop="1" thickBot="1">
       <c r="H143" s="9" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="I143" s="9" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
     </row>
     <row r="144" spans="3:9" ht="16" thickTop="1"/>

</xml_diff>

<commit_message>
code for July 2015 rerun
</commit_message>
<xml_diff>
--- a/project management/gantt chart - moved to drive.xlsx
+++ b/project management/gantt chart - moved to drive.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28320" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="319">
   <si>
     <t>TAU data</t>
   </si>
@@ -936,7 +936,46 @@
     <t>Knowledge Bank Synapse ID - data</t>
   </si>
   <si>
-    <t>`</t>
+    <t>syn4239736</t>
+  </si>
+  <si>
+    <t>AMP-AD_MayoBB_UFL-Mayo-ISB_IlluminaHiSeq2000_TCX_GeneCounts_JulyRerun.txt.gz</t>
+  </si>
+  <si>
+    <t>AMP-AD_MayoBB_UFL-Mayo-ISB_IlluminaHiSeq2000_TCX_TranscriptCounts_JulyRerun.txt.gz</t>
+  </si>
+  <si>
+    <t>AMP-AD_MayoBB_UFL-Mayo-ISB_IlluminaHiSeq2000_TCX_GeneCounts_Normalized_JulyRerun.txt.gz</t>
+  </si>
+  <si>
+    <t>AMP-AD_MayoBB_UFL-Mayo-ISB_IlluminaHiSeq2000_TCX_TranscriptCounts_Normalized_JulyRerun.txt.gz</t>
+  </si>
+  <si>
+    <t>syn4650257</t>
+  </si>
+  <si>
+    <t>syn4650258</t>
+  </si>
+  <si>
+    <t>syn4650265</t>
+  </si>
+  <si>
+    <t>syn4650430</t>
+  </si>
+  <si>
+    <t>RNA-Seq RERUN</t>
+  </si>
+  <si>
+    <t>AMP-AD_SampleSwap_UFL-Mayo-ISB_IlluminaHiSeq2000_dIPFC_Rush-Broad-SS_GeneCounts_JulyRerun.txt.gz</t>
+  </si>
+  <si>
+    <t>AMP-AD_SampleSwap_UFL-Mayo-ISB_IlluminaHiSeq2000_dIPFC_Rush-Broad-SS_geneCounts_normalized_JulyRerun.txt.gz</t>
+  </si>
+  <si>
+    <t>AMP-AD_SampleSwap_UFL-Mayo-ISB_IlluminaHiSeq2000_dIPFC_Rush-Broad-SS_TranscriptCounts_JulyRerun.txt.gz</t>
+  </si>
+  <si>
+    <t>AMP-AD_SampleSwap_UFL-Mayo-ISB_IlluminaHiSeq2000_dIPFC_Rush-Broad-SS_TranscriptCounts_Normalized_JulyRerun.txt.gz</t>
   </si>
 </sst>
 </file>
@@ -1094,7 +1133,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="123">
+  <cellStyleXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1218,8 +1257,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="17" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1264,8 +1305,10 @@
     <xf numFmtId="17" fontId="9" fillId="7" borderId="0" xfId="81" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="17" fontId="1" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="81" applyFill="1"/>
+    <xf numFmtId="17" fontId="9" fillId="0" borderId="0" xfId="81" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="123">
+  <cellStyles count="125">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Check Cell" xfId="56" builtinId="23"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -1373,6 +1416,8 @@
     <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="121" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="123" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="81" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="24" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
@@ -3925,13 +3970,13 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I144"/>
+  <dimension ref="A1:I162"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E124" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F138" sqref="F138"/>
+      <selection pane="bottomRight" activeCell="C148" sqref="C148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4043,9 +4088,6 @@
       <c r="I9" s="7"/>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" t="s">
-        <v>305</v>
-      </c>
       <c r="E10" s="1"/>
       <c r="H10" s="5"/>
       <c r="I10" s="7"/>
@@ -5128,7 +5170,7 @@
         <v>161</v>
       </c>
       <c r="G118" t="s">
-        <v>8</v>
+        <v>314</v>
       </c>
       <c r="I118" s="4" t="s">
         <v>178</v>
@@ -5157,38 +5199,38 @@
     </row>
     <row r="121" spans="1:9" s="23" customFormat="1">
       <c r="C121" s="23" t="s">
-        <v>266</v>
+        <v>310</v>
       </c>
       <c r="E121" s="25"/>
       <c r="H121" s="23" t="s">
-        <v>265</v>
+        <v>306</v>
       </c>
     </row>
     <row r="122" spans="1:9" s="23" customFormat="1">
       <c r="C122" s="23" t="s">
-        <v>267</v>
+        <v>312</v>
       </c>
       <c r="E122" s="25"/>
       <c r="H122" s="23" t="s">
-        <v>268</v>
+        <v>308</v>
       </c>
     </row>
     <row r="123" spans="1:9" s="23" customFormat="1">
       <c r="C123" s="23" t="s">
-        <v>269</v>
+        <v>311</v>
       </c>
       <c r="E123" s="25"/>
       <c r="H123" s="23" t="s">
-        <v>272</v>
+        <v>307</v>
       </c>
     </row>
     <row r="124" spans="1:9" s="23" customFormat="1" ht="16" thickBot="1">
       <c r="C124" s="23" t="s">
-        <v>270</v>
+        <v>313</v>
       </c>
       <c r="E124" s="25"/>
       <c r="H124" s="23" t="s">
-        <v>271</v>
+        <v>309</v>
       </c>
     </row>
     <row r="125" spans="1:9" s="9" customFormat="1" ht="17" thickTop="1" thickBot="1">
@@ -5199,150 +5241,295 @@
         <v>183</v>
       </c>
     </row>
-    <row r="126" spans="1:9" ht="17" thickTop="1" thickBot="1"/>
-    <row r="127" spans="1:9" s="9" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="E127" s="10">
+    <row r="126" spans="1:9" ht="16" thickTop="1"/>
+    <row r="127" spans="1:9" s="4" customFormat="1">
+      <c r="D127" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="E127" s="6">
+        <v>42125</v>
+      </c>
+      <c r="F127" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="G127" t="s">
+        <v>8</v>
+      </c>
+      <c r="I127" s="4" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" s="28" customFormat="1">
+      <c r="C128" s="28" t="s">
+        <v>264</v>
+      </c>
+      <c r="E128" s="29"/>
+      <c r="H128" s="28" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="129" spans="3:9" s="8" customFormat="1">
+      <c r="C129" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="E129" s="24"/>
+      <c r="H129" s="8" t="s">
+        <v>250</v>
+      </c>
+      <c r="I129" s="8" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="130" spans="3:9" s="28" customFormat="1">
+      <c r="C130" s="28" t="s">
+        <v>266</v>
+      </c>
+      <c r="E130" s="29"/>
+      <c r="H130" s="28" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="131" spans="3:9" s="28" customFormat="1">
+      <c r="C131" s="28" t="s">
+        <v>267</v>
+      </c>
+      <c r="E131" s="29"/>
+      <c r="H131" s="28" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="132" spans="3:9" s="28" customFormat="1">
+      <c r="C132" s="28" t="s">
+        <v>269</v>
+      </c>
+      <c r="E132" s="29"/>
+      <c r="H132" s="28" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="133" spans="3:9" s="28" customFormat="1" ht="16" thickBot="1">
+      <c r="C133" s="28" t="s">
+        <v>270</v>
+      </c>
+      <c r="E133" s="29"/>
+      <c r="H133" s="28" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="134" spans="3:9" s="9" customFormat="1" ht="17" thickTop="1" thickBot="1">
+      <c r="E134" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="H134" s="9" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="135" spans="3:9" ht="17" thickTop="1" thickBot="1"/>
+    <row r="136" spans="3:9" s="9" customFormat="1" ht="17" thickTop="1" thickBot="1">
+      <c r="E136" s="10">
         <v>42401</v>
       </c>
-      <c r="F127" s="9" t="s">
+      <c r="F136" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="I127" s="9" t="s">
+      <c r="I136" s="9" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="128" spans="1:9" ht="16" thickTop="1">
-      <c r="E128" s="1"/>
-    </row>
-    <row r="129" spans="3:9" s="4" customFormat="1">
-      <c r="D129" s="4" t="s">
+    <row r="137" spans="3:9" ht="16" thickTop="1">
+      <c r="E137" s="1"/>
+    </row>
+    <row r="138" spans="3:9" s="4" customFormat="1">
+      <c r="D138" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="E129" s="6">
+      <c r="E138" s="6">
         <v>42125</v>
       </c>
-      <c r="F129" s="4" t="s">
+      <c r="F138" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="G129" s="4" t="s">
+      <c r="G138" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I129" s="4" t="s">
+      <c r="I138" s="4" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="130" spans="3:9" s="23" customFormat="1">
-      <c r="C130" s="23" t="s">
+    <row r="139" spans="3:9" s="23" customFormat="1">
+      <c r="C139" s="23" t="s">
         <v>248</v>
       </c>
-      <c r="H130" s="23" t="s">
+      <c r="H139" s="23" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="131" spans="3:9" s="8" customFormat="1">
-      <c r="C131" s="8" t="s">
+    <row r="140" spans="3:9" s="8" customFormat="1">
+      <c r="C140" s="8" t="s">
         <v>245</v>
       </c>
-      <c r="H131" s="8" t="s">
+      <c r="H140" s="8" t="s">
         <v>201</v>
       </c>
-      <c r="I131" s="8" t="s">
+      <c r="I140" s="8" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="132" spans="3:9" s="23" customFormat="1">
-      <c r="C132" s="23" t="s">
+    <row r="141" spans="3:9" s="23" customFormat="1">
+      <c r="C141" s="23" t="s">
         <v>257</v>
       </c>
-      <c r="H132" s="23" t="s">
+      <c r="H141" s="23" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="133" spans="3:9" s="23" customFormat="1">
-      <c r="C133" s="23" t="s">
+    <row r="142" spans="3:9" s="23" customFormat="1">
+      <c r="C142" s="23" t="s">
         <v>258</v>
       </c>
-      <c r="H133" s="23" t="s">
+      <c r="H142" s="23" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="134" spans="3:9" s="23" customFormat="1">
-      <c r="C134" s="23" t="s">
+    <row r="143" spans="3:9" s="23" customFormat="1">
+      <c r="C143" s="23" t="s">
         <v>260</v>
       </c>
-      <c r="H134" s="23" t="s">
+      <c r="H143" s="23" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="135" spans="3:9" s="23" customFormat="1" ht="16" thickBot="1">
-      <c r="C135" s="23" t="s">
+    <row r="144" spans="3:9" s="23" customFormat="1" ht="16" thickBot="1">
+      <c r="C144" s="23" t="s">
         <v>261</v>
       </c>
-      <c r="H135" s="23" t="s">
+      <c r="H144" s="23" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="136" spans="3:9" s="9" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="E136" s="9" t="s">
+    <row r="145" spans="4:9" s="9" customFormat="1" ht="17" thickTop="1" thickBot="1">
+      <c r="E145" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="H136" s="9" t="s">
+      <c r="H145" s="9" t="s">
         <v>208</v>
       </c>
-      <c r="I136" s="9" t="s">
+      <c r="I145" s="9" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="137" spans="3:9" ht="17" thickTop="1" thickBot="1"/>
-    <row r="138" spans="3:9" s="9" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="D138" s="9" t="s">
+    <row r="146" spans="4:9" ht="16" thickTop="1"/>
+    <row r="147" spans="4:9" s="4" customFormat="1">
+      <c r="D147" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="E147" s="6">
+        <v>42125</v>
+      </c>
+      <c r="F147" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="G147" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="I147" s="4" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="148" spans="4:9" s="23" customFormat="1">
+      <c r="H148" s="23" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="149" spans="4:9" s="8" customFormat="1">
+      <c r="H149" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="I149" s="8" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="150" spans="4:9" s="23" customFormat="1">
+      <c r="H150" s="23" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="151" spans="4:9" s="23" customFormat="1">
+      <c r="H151" s="23" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="152" spans="4:9" s="23" customFormat="1">
+      <c r="H152" s="23" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="153" spans="4:9" s="23" customFormat="1" ht="16" thickBot="1">
+      <c r="H153" s="23" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="154" spans="4:9" s="9" customFormat="1" ht="17" thickTop="1" thickBot="1">
+      <c r="E154" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="H154" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="I154" s="9" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="155" spans="4:9" ht="17" thickTop="1" thickBot="1"/>
+    <row r="156" spans="4:9" s="9" customFormat="1" ht="17" thickTop="1" thickBot="1">
+      <c r="D156" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="E138" s="9" t="s">
+      <c r="E156" s="9" t="s">
         <v>204</v>
       </c>
-      <c r="F138" s="9" t="s">
+      <c r="F156" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="G138" s="9" t="s">
+      <c r="G156" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="I138" s="9" t="s">
+      <c r="I156" s="9" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="139" spans="3:9" s="9" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="H139" s="9" t="s">
+    <row r="157" spans="4:9" s="9" customFormat="1" ht="17" thickTop="1" thickBot="1">
+      <c r="H157" s="9" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="140" spans="3:9" s="9" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="H140" s="9" t="s">
+    <row r="158" spans="4:9" s="9" customFormat="1" ht="17" thickTop="1" thickBot="1">
+      <c r="H158" s="9" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="141" spans="3:9" s="9" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="H141" s="9" t="s">
+    <row r="159" spans="4:9" s="9" customFormat="1" ht="17" thickTop="1" thickBot="1">
+      <c r="H159" s="9" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="142" spans="3:9" s="9" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="H142" s="9" t="s">
+    <row r="160" spans="4:9" s="9" customFormat="1" ht="17" thickTop="1" thickBot="1">
+      <c r="H160" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="I142" s="9" t="s">
+      <c r="I160" s="9" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="143" spans="3:9" s="9" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="H143" s="9" t="s">
+    <row r="161" spans="8:9" s="9" customFormat="1" ht="17" thickTop="1" thickBot="1">
+      <c r="H161" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="I143" s="9" t="s">
+      <c r="I161" s="9" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="144" spans="3:9" ht="16" thickTop="1"/>
+    <row r="162" spans="8:9" ht="16" thickTop="1"/>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <hyperlinks>

</xml_diff>